<commit_message>
import from excel finished
rowData is imported
</commit_message>
<xml_diff>
--- a/AntiLaundering/View/Download/CustomerTransact.xlsx
+++ b/AntiLaundering/View/Download/CustomerTransact.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\ACT_Masters\Thesis_MS_MSC632\_Capstone_Project\DataCollection\AntiMoneyLaundering\AntiLaundering\View\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF568A7-C0DA-43DC-97EB-105D794DAB28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1573CB2A-7540-48B9-B5B4-D2CE494897B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{82231500-2076-4EBB-ABBB-55FE3E1BCD36}"/>
   </bookViews>
   <sheets>
-    <sheet name="CustomerTransact" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,34 +25,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>CustomerID</t>
-  </si>
-  <si>
-    <t>CustomerAccount</t>
-  </si>
-  <si>
-    <t>BusinessDate</t>
-  </si>
-  <si>
-    <t>DebitedDateTime</t>
-  </si>
-  <si>
-    <t>TransactionAmount</t>
-  </si>
-  <si>
-    <t>TransactionType</t>
-  </si>
-  <si>
-    <t>MobileBanking</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="19">
+  <si>
+    <t>TXN_ID</t>
+  </si>
+  <si>
+    <t>DEBIT_CUSTOMER</t>
+  </si>
+  <si>
+    <t>CREDIT_CUSTOMER</t>
+  </si>
+  <si>
+    <t>DEBIT_ACCT_NO</t>
+  </si>
+  <si>
+    <t>CREDIT_ACCT_NO</t>
+  </si>
+  <si>
+    <t>BUSINESS_DATE</t>
+  </si>
+  <si>
+    <t>TRANSACTION_BY</t>
+  </si>
+  <si>
+    <t>DEBIT_CURRENCY</t>
+  </si>
+  <si>
+    <t>USD_EQUIV_BALANCE</t>
+  </si>
+  <si>
+    <t>CREDIT_AMOUNT</t>
+  </si>
+  <si>
+    <t>AGE</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>REGIONNAME</t>
+  </si>
+  <si>
+    <t>DISTRICTNAME</t>
+  </si>
+  <si>
+    <t>MOBILEBANKING</t>
+  </si>
+  <si>
+    <t>ETB</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>OROMIYA</t>
+  </si>
+  <si>
+    <t>BALE ROBE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +106,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -95,11 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,24 +458,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0B8AEB-77E7-4A8D-A86C-2F80983A025B}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053DCD99-7EA2-4C14-ACFF-0A713E11837D}">
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,29 +502,559 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3597904</v>
       </c>
       <c r="C2" s="2">
-        <v>44811</v>
-      </c>
-      <c r="D2" s="3">
-        <v>44811.570833333331</v>
-      </c>
-      <c r="E2">
-        <v>50000</v>
-      </c>
-      <c r="F2" t="s">
+        <v>4540228</v>
+      </c>
+      <c r="D2" s="2">
+        <v>14409990</v>
+      </c>
+      <c r="E2" s="2">
+        <v>13341160</v>
+      </c>
+      <c r="F2" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2">
+        <v>56.64</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3000</v>
+      </c>
+      <c r="K2" s="2">
+        <v>39</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2841945</v>
+      </c>
+      <c r="C3" s="2">
+        <v>537639</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10459103</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12551427</v>
+      </c>
+      <c r="F3" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2">
+        <v>98.17</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5200</v>
+      </c>
+      <c r="K3" s="2">
+        <v>33</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1900885</v>
+      </c>
+      <c r="C4" s="2">
+        <v>537574</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12470087</v>
+      </c>
+      <c r="E4" s="2">
+        <v>11642884</v>
+      </c>
+      <c r="F4" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4000</v>
+      </c>
+      <c r="K4" s="2">
+        <v>48</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3027476</v>
+      </c>
+      <c r="C5" s="2">
+        <v>537642</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10459113</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12741433</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2">
+        <v>75.510000000000005</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4000</v>
+      </c>
+      <c r="K5" s="2">
+        <v>45</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4471774</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2206121</v>
+      </c>
+      <c r="D6" s="2">
+        <v>11932128</v>
+      </c>
+      <c r="E6" s="2">
+        <v>14323410</v>
+      </c>
+      <c r="F6" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2">
+        <v>60.79</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3220</v>
+      </c>
+      <c r="K6" s="2">
+        <v>28</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2864377</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3477870</v>
+      </c>
+      <c r="D7" s="2">
+        <v>13212740</v>
+      </c>
+      <c r="E7" s="2">
+        <v>12573947</v>
+      </c>
+      <c r="F7" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <v>755.14</v>
+      </c>
+      <c r="J7" s="2">
+        <v>40000</v>
+      </c>
+      <c r="K7" s="2">
+        <v>44</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2864377</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3477870</v>
+      </c>
+      <c r="D8" s="2">
+        <v>13212740</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12573947</v>
+      </c>
+      <c r="F8" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1887.86</v>
+      </c>
+      <c r="J8" s="2">
+        <v>100000</v>
+      </c>
+      <c r="K8" s="2">
+        <v>44</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4434416</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2336937</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12054664</v>
+      </c>
+      <c r="E9" s="2">
+        <v>14277785</v>
+      </c>
+      <c r="F9" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2">
+        <v>409.67</v>
+      </c>
+      <c r="J9" s="2">
+        <v>21700</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4431595</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3542632</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13281863</v>
+      </c>
+      <c r="E10" s="2">
+        <v>14274387</v>
+      </c>
+      <c r="F10" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2">
+        <v>566.36</v>
+      </c>
+      <c r="J10" s="2">
+        <v>30000</v>
+      </c>
+      <c r="K10" s="2">
+        <v>32</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1091663</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1600186</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12788075</v>
+      </c>
+      <c r="E11" s="2">
+        <v>14464776</v>
+      </c>
+      <c r="F11" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2">
+        <v>566.36</v>
+      </c>
+      <c r="J11" s="2">
+        <v>30000</v>
+      </c>
+      <c r="K11" s="2">
+        <v>31</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4479802</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1198670</v>
+      </c>
+      <c r="D12" s="2">
+        <v>11014040</v>
+      </c>
+      <c r="E12" s="2">
+        <v>14333214</v>
+      </c>
+      <c r="F12" s="3">
+        <v>44803</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2">
+        <v>56.64</v>
+      </c>
+      <c r="J12" s="2">
+        <v>3000</v>
+      </c>
+      <c r="K12" s="2">
+        <v>34</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4886887</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2353794</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12070934</v>
+      </c>
+      <c r="E13" s="2">
+        <v>14861426</v>
+      </c>
+      <c r="F13" s="3">
+        <v>44802</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2">
+        <v>321</v>
+      </c>
+      <c r="J13" s="2">
+        <v>17000</v>
+      </c>
+      <c r="K13" s="2">
+        <v>42</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>